<commit_message>
thorough updates of Bwaise module results
</commit_message>
<xml_diff>
--- a/exposan/bwaise/comparison/baseline/Bwaise_sanitation_outputs_baselineA.xlsx
+++ b/exposan/bwaise/comparison/baseline/Bwaise_sanitation_outputs_baselineA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/es/exposan/bwaise/comparison/baseline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_305B40670E71B04B21CEEDC7EE3FDD3B4993FAA8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CEF9016-88CE-044C-BEEB-3B0E6CAF5E92}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_305B40670E71B04B21CEEDC7EE3FDD3B4993FAA8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3C71428-947A-EB4E-89AD-6C6C795C24F0}"/>
   <bookViews>
     <workbookView xWindow="860" yWindow="1200" windowWidth="27700" windowHeight="19480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -438,8 +438,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -605,7 +606,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -627,10 +628,11 @@
     <xf numFmtId="164" fontId="3" fillId="2" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="5" xfId="2" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -973,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G20" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="G35" workbookViewId="0">
+      <selection activeCell="J60" sqref="J60:N61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2431,7 +2433,7 @@
       <c r="K56" s="10">
         <v>5.0432063842220418E-2</v>
       </c>
-      <c r="L56" s="19">
+      <c r="L56" s="17">
         <v>5.0432063842220418E-2</v>
       </c>
       <c r="M56" s="10">
@@ -2478,19 +2480,19 @@
       <c r="I60" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="J60" s="4">
+      <c r="J60" s="18">
         <v>59.029808894462683</v>
       </c>
-      <c r="K60" s="17">
+      <c r="K60" s="19">
         <v>59.029808894462683</v>
       </c>
       <c r="L60" s="20">
         <v>59.029808894462683</v>
       </c>
-      <c r="M60" s="17">
+      <c r="M60" s="19">
         <v>59.029808894462683</v>
       </c>
-      <c r="N60" s="4">
+      <c r="N60" s="18">
         <v>59.029808894462683</v>
       </c>
     </row>
@@ -2498,19 +2500,19 @@
       <c r="I61" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="J61" s="4">
+      <c r="J61" s="18">
         <v>14.206547126983351</v>
       </c>
-      <c r="K61" s="17">
+      <c r="K61" s="19">
         <v>14.206547126983351</v>
       </c>
-      <c r="L61" s="18">
+      <c r="L61" s="21">
         <v>14.206547126983351</v>
       </c>
-      <c r="M61" s="17">
+      <c r="M61" s="19">
         <v>14.206547126983351</v>
       </c>
-      <c r="N61" s="4">
+      <c r="N61" s="18">
         <v>14.206547126983351</v>
       </c>
     </row>

</xml_diff>